<commit_message>
Updated Sales Forecast. Pricing is now Php100.00 and Php28.50, which gives us revenue of Php70.00 and Php20.00
</commit_message>
<xml_diff>
--- a/Business Plan Documents/YPS Sales Forecast.xlsx
+++ b/Business Plan Documents/YPS Sales Forecast.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8340" tabRatio="694"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="19560" windowHeight="8340" tabRatio="694"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Forecast (Year 1)" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Microsoft</author>
+    <author>Josh</author>
   </authors>
   <commentList>
     <comment ref="B10" authorId="0" shapeId="0">
@@ -39,6 +40,32 @@
             <family val="2"/>
           </rPr>
           <t>Totals are calculated automatically.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A13" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="7"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pricing is Php100.00, but 30% goes to Operating Expenses of Google</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="7"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pricing is Php28.50, but 30% goes to Operating Expenses of Google</t>
         </r>
       </text>
     </comment>
@@ -317,7 +344,7 @@
     <numFmt numFmtId="166" formatCode="yyyy"/>
     <numFmt numFmtId="167" formatCode="[$-3409]dd\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -365,6 +392,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -685,10 +718,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,8 +1007,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -998,7 +1031,7 @@
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="23"/>
@@ -1353,40 +1386,40 @@
         <v>0</v>
       </c>
       <c r="B13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="9"/>
@@ -1401,55 +1434,55 @@
       </c>
       <c r="B14" s="3">
         <f>B12*B13</f>
-        <v>150000</v>
+        <v>105000</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:S14" si="3">C12*C13</f>
-        <v>250000</v>
+        <v>175000</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>250000</v>
+        <v>175000</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>350000</v>
+        <v>245000</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
-        <v>375000</v>
+        <v>262500</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
-        <v>625000</v>
+        <v>437500</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="3"/>
-        <v>937500</v>
+        <v>656250</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="3"/>
-        <v>1312500</v>
+        <v>918750</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="3"/>
-        <v>900000</v>
+        <v>630000</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="3"/>
-        <v>1500000</v>
+        <v>1050000</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="3"/>
-        <v>1500000</v>
+        <v>1050000</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="3"/>
-        <v>2100000</v>
+        <v>1470000</v>
       </c>
       <c r="N14" s="22">
         <f>SUM(B14:M14)</f>
-        <v>10250000</v>
+        <v>7175000</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="51">
@@ -2385,55 +2418,55 @@
       </c>
       <c r="B36" s="60">
         <f>(B10+B14+B18+B22+B26+B30+B34)</f>
-        <v>206050</v>
+        <v>161050</v>
       </c>
       <c r="C36" s="60">
         <f t="shared" ref="C36:S36" si="15">(C10+C14+C18+C22+C26+C30+C34)</f>
-        <v>343210</v>
+        <v>268210</v>
       </c>
       <c r="D36" s="60">
         <f t="shared" si="15"/>
-        <v>344450</v>
+        <v>269450</v>
       </c>
       <c r="E36" s="60">
         <f t="shared" si="15"/>
-        <v>479750</v>
+        <v>374750</v>
       </c>
       <c r="F36" s="60">
         <f t="shared" si="15"/>
-        <v>514815</v>
+        <v>402315</v>
       </c>
       <c r="G36" s="60">
         <f t="shared" si="15"/>
-        <v>862425</v>
+        <v>674925</v>
       </c>
       <c r="H36" s="60">
         <f t="shared" si="15"/>
-        <v>1237425</v>
+        <v>956175</v>
       </c>
       <c r="I36" s="60">
         <f t="shared" si="15"/>
-        <v>1725675</v>
+        <v>1331925</v>
       </c>
       <c r="J36" s="60">
         <f t="shared" si="15"/>
-        <v>1188600</v>
+        <v>918600</v>
       </c>
       <c r="K36" s="60">
         <f t="shared" si="15"/>
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="L36" s="60">
         <f t="shared" si="15"/>
-        <v>1969800</v>
+        <v>1519800</v>
       </c>
       <c r="M36" s="60">
         <f t="shared" si="15"/>
-        <v>2748760</v>
+        <v>2118760</v>
       </c>
       <c r="N36" s="61">
         <f>SUM(B36:M36)</f>
-        <v>13590760</v>
+        <v>10515760</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="51">
@@ -2491,7 +2524,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2514,7 +2547,7 @@
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="23"/>
@@ -2869,40 +2902,40 @@
         <v>0</v>
       </c>
       <c r="B13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="9"/>
@@ -2917,55 +2950,55 @@
       </c>
       <c r="B14" s="3">
         <f>B12*B13</f>
-        <v>600000</v>
+        <v>420000</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:S14" si="3">C12*C13</f>
-        <v>920000</v>
+        <v>644000</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>1080000</v>
+        <v>756000</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>1400000</v>
+        <v>980000</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
-        <v>750000</v>
+        <v>525000</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
-        <v>1250000</v>
+        <v>875000</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="3"/>
-        <v>1875000</v>
+        <v>1312500</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="3"/>
-        <v>2625000</v>
+        <v>1837500</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="3"/>
-        <v>1350000</v>
+        <v>945000</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="3"/>
-        <v>2250000</v>
+        <v>1575000</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="3"/>
-        <v>2250000</v>
+        <v>1575000</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="3"/>
-        <v>3150000</v>
+        <v>2205000</v>
       </c>
       <c r="N14" s="22">
         <f>SUM(B14:M14)</f>
-        <v>19500000</v>
+        <v>13650000</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="51">
@@ -3901,55 +3934,55 @@
       </c>
       <c r="B36" s="60">
         <f>(B10+B14+B18+B22+B26+B30+B34)</f>
-        <v>816140</v>
+        <v>636140</v>
       </c>
       <c r="C36" s="60">
         <f t="shared" ref="C36:S36" si="15">(C10+C14+C18+C22+C26+C30+C34)</f>
-        <v>1250960</v>
+        <v>974960</v>
       </c>
       <c r="D36" s="60">
         <f t="shared" si="15"/>
-        <v>1468680</v>
+        <v>1144680</v>
       </c>
       <c r="E36" s="60">
         <f t="shared" si="15"/>
-        <v>1901640</v>
+        <v>1481640</v>
       </c>
       <c r="F36" s="60">
         <f t="shared" si="15"/>
-        <v>1023430</v>
+        <v>798430</v>
       </c>
       <c r="G36" s="60">
         <f t="shared" si="15"/>
-        <v>1710290</v>
+        <v>1335290</v>
       </c>
       <c r="H36" s="60">
         <f t="shared" si="15"/>
-        <v>2460290</v>
+        <v>1897790</v>
       </c>
       <c r="I36" s="60">
         <f t="shared" si="15"/>
-        <v>3436790</v>
+        <v>2649290</v>
       </c>
       <c r="J36" s="60">
         <f t="shared" si="15"/>
-        <v>1776740</v>
+        <v>1371740</v>
       </c>
       <c r="K36" s="60">
         <f t="shared" si="15"/>
-        <v>2948540</v>
+        <v>2273540</v>
       </c>
       <c r="L36" s="60">
         <f t="shared" si="15"/>
-        <v>2948540</v>
+        <v>2273540</v>
       </c>
       <c r="M36" s="60">
         <f t="shared" si="15"/>
-        <v>4118100</v>
+        <v>3173100</v>
       </c>
       <c r="N36" s="61">
         <f>SUM(B36:M36)</f>
-        <v>25860140</v>
+        <v>20010140</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="51">
@@ -4006,7 +4039,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4029,7 +4062,7 @@
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="23"/>
@@ -4384,40 +4417,40 @@
         <v>0</v>
       </c>
       <c r="B13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="9"/>
@@ -4432,55 +4465,55 @@
       </c>
       <c r="B14" s="3">
         <f>B12*B13</f>
-        <v>900000</v>
+        <v>630000</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:S14" si="3">C12*C13</f>
-        <v>1380000</v>
+        <v>966000</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>1620000</v>
+        <v>1134000</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>2100000</v>
+        <v>1470000</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
-        <v>1350000</v>
+        <v>945000</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
-        <v>2250000</v>
+        <v>1575000</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="3"/>
-        <v>3375000</v>
+        <v>2362500</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="3"/>
-        <v>4725000</v>
+        <v>3307500</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="3"/>
-        <v>2250000</v>
+        <v>1575000</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="3"/>
-        <v>3750000</v>
+        <v>2625000</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="3"/>
-        <v>3750000</v>
+        <v>2625000</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="3"/>
-        <v>5250000</v>
+        <v>3675000</v>
       </c>
       <c r="N14" s="22">
         <f>SUM(B14:M14)</f>
-        <v>32700000</v>
+        <v>22890000</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="51">
@@ -5416,55 +5449,55 @@
       </c>
       <c r="B36" s="60">
         <f>(B10+B14+B18+B22+B26+B30+B34)</f>
-        <v>1223280</v>
+        <v>953280</v>
       </c>
       <c r="C36" s="60">
         <f t="shared" ref="C36:S36" si="15">(C10+C14+C18+C22+C26+C30+C34)</f>
-        <v>1874580</v>
+        <v>1460580</v>
       </c>
       <c r="D36" s="60">
         <f t="shared" si="15"/>
-        <v>2200540</v>
+        <v>1714540</v>
       </c>
       <c r="E36" s="60">
         <f t="shared" si="15"/>
-        <v>2930580</v>
+        <v>2300580</v>
       </c>
       <c r="F36" s="60">
         <f t="shared" si="15"/>
-        <v>1836470</v>
+        <v>1431470</v>
       </c>
       <c r="G36" s="60">
         <f t="shared" si="15"/>
-        <v>3065530</v>
+        <v>2390530</v>
       </c>
       <c r="H36" s="60">
         <f t="shared" si="15"/>
-        <v>4415530</v>
+        <v>3403030</v>
       </c>
       <c r="I36" s="60">
         <f t="shared" si="15"/>
-        <v>6173230</v>
+        <v>4755730</v>
       </c>
       <c r="J36" s="60">
         <f t="shared" si="15"/>
-        <v>2950780</v>
+        <v>2275780</v>
       </c>
       <c r="K36" s="60">
         <f t="shared" si="15"/>
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="L36" s="60">
         <f t="shared" si="15"/>
-        <v>4903780</v>
+        <v>3778780</v>
       </c>
       <c r="M36" s="60">
         <f t="shared" si="15"/>
-        <v>6854540</v>
+        <v>5279540</v>
       </c>
       <c r="N36" s="61">
         <f>SUM(B36:M36)</f>
-        <v>43332620</v>
+        <v>33522620</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="51">
@@ -5521,7 +5554,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5544,7 +5577,7 @@
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="23"/>
@@ -5899,40 +5932,40 @@
         <v>0</v>
       </c>
       <c r="B13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="H13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M13" s="32">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="N13" s="33"/>
       <c r="O13" s="9"/>
@@ -5947,55 +5980,55 @@
       </c>
       <c r="B14" s="3">
         <f>B12*B13</f>
-        <v>1500000</v>
+        <v>1050000</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ref="C14:S14" si="3">C12*C13</f>
-        <v>2300000</v>
+        <v>1610000</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="3"/>
-        <v>2700000</v>
+        <v>1890000</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="3"/>
-        <v>3500000</v>
+        <v>2450000</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="3"/>
-        <v>1875000</v>
+        <v>1312500</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="3"/>
-        <v>3125000</v>
+        <v>2187500</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="3"/>
-        <v>4687500</v>
+        <v>3281250</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="3"/>
-        <v>6562500</v>
+        <v>4593750</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="3"/>
-        <v>3037500</v>
+        <v>2126250</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="3"/>
-        <v>5062500</v>
+        <v>3543750</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="3"/>
-        <v>5062500</v>
+        <v>3543750</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="3"/>
-        <v>7087499.9999999981</v>
+        <v>4961249.9999999991</v>
       </c>
       <c r="N14" s="22">
         <f>SUM(B14:M14)</f>
-        <v>46500000</v>
+        <v>32550000</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="51">
@@ -6931,55 +6964,55 @@
       </c>
       <c r="B36" s="60">
         <f>(B10+B14+B18+B22+B26+B30+B34)</f>
-        <v>2036320</v>
+        <v>1586320</v>
       </c>
       <c r="C36" s="60">
         <f t="shared" ref="C36:S36" si="15">(C10+C14+C18+C22+C26+C30+C34)</f>
-        <v>3120580</v>
+        <v>2430580</v>
       </c>
       <c r="D36" s="60">
         <f t="shared" si="15"/>
-        <v>3663020</v>
+        <v>2853020</v>
       </c>
       <c r="E36" s="60">
         <f t="shared" si="15"/>
-        <v>4745420</v>
+        <v>3695420</v>
       </c>
       <c r="F36" s="60">
         <f t="shared" si="15"/>
-        <v>2548035</v>
+        <v>1985535</v>
       </c>
       <c r="G36" s="60">
         <f t="shared" si="15"/>
-        <v>4251645</v>
+        <v>3314145</v>
       </c>
       <c r="H36" s="60">
         <f t="shared" si="15"/>
-        <v>6126645</v>
+        <v>4720395</v>
       </c>
       <c r="I36" s="60">
         <f t="shared" si="15"/>
-        <v>8567895</v>
+        <v>6599145</v>
       </c>
       <c r="J36" s="60">
         <f t="shared" si="15"/>
-        <v>3978345</v>
+        <v>3067095</v>
       </c>
       <c r="K36" s="60">
         <f t="shared" si="15"/>
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="L36" s="60">
         <f t="shared" si="15"/>
-        <v>6614895</v>
+        <v>5096145</v>
       </c>
       <c r="M36" s="60">
         <f t="shared" si="15"/>
-        <v>9249204.9999999981</v>
+        <v>7122954.9999999991</v>
       </c>
       <c r="N36" s="61">
         <f>SUM(B36:M36)</f>
-        <v>61516900</v>
+        <v>47566900</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="51">
@@ -7051,10 +7084,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="74"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="65">
         <v>5000000</v>
       </c>

</xml_diff>